<commit_message>
Correción y adición de información
</commit_message>
<xml_diff>
--- a/2-Analisis_de_Riesgos.xlsx
+++ b/2-Analisis_de_Riesgos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\Ejercicio Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF49858-F12B-461E-94FC-1CC7DBB058C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C55A31-433E-4BC0-A34B-35FEB12D8703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Riesgo</t>
   </si>
@@ -107,15 +107,6 @@
     <t>Se definen las pruebas a realizar de acuerdo a su criticidad.</t>
   </si>
   <si>
-    <t>Compatibilidad entre navegadores</t>
-  </si>
-  <si>
-    <t>Existe el riesgo que el producto de software no sea compatible con algunos navegadores</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
     <t>Usabilidad</t>
   </si>
   <si>
@@ -215,13 +206,19 @@
     <t>Proyecto</t>
   </si>
   <si>
-    <t>Realizar pruebas de compatibilidad en los navegadores requeridos por el cliente (Chrome, Firefox) y en las versiones correctas detalladas en  el documento de criterios técnicos</t>
-  </si>
-  <si>
     <t>Pruebas de usabilidad</t>
   </si>
   <si>
     <t>El aplicativo no responde a escenarios de fallos</t>
+  </si>
+  <si>
+    <t>Ingreso de caracteres especiales</t>
+  </si>
+  <si>
+    <t>El ingreso de caracteres especiales supone un riesgo para la integridad de los datos, teniendo en cuenta que los atacantes pueden utilizar combinaciones para alterar la información.</t>
+  </si>
+  <si>
+    <t>Verificar que en el campo de búsqueda no se puedan ingresar caracteres especiales - Prueba de seguridad</t>
   </si>
 </sst>
 </file>
@@ -349,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -553,6 +550,32 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -562,7 +585,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,9 +630,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -645,6 +665,15 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1017,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1043,40 +1072,40 @@
   <sheetData>
     <row r="1" spans="2:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="G2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>58</v>
+      <c r="B3" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>9</v>
@@ -1091,20 +1120,20 @@
         <f>F3*G3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>51</v>
+      <c r="I3" s="22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F4" s="11">
         <v>3</v>
@@ -1116,14 +1145,14 @@
         <f>F4*G4</f>
         <v>3</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>54</v>
+      <c r="I4" s="17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
@@ -1141,14 +1170,14 @@
         <f>F5*G5</f>
         <v>3</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>55</v>
+      <c r="I5" s="23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
@@ -1166,20 +1195,20 @@
         <f>F6*G6</f>
         <v>2</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
@@ -1191,91 +1220,89 @@
         <f>F7*G7</f>
         <v>6</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="35"/>
-      <c r="C8" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="25" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="21">
-        <v>3</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="20">
+        <v>3</v>
+      </c>
+      <c r="G8" s="20">
         <v>1</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="20">
         <f t="shared" ref="H8:H13" si="0">F8*G8</f>
         <v>3</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+    <row r="9" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="11">
+        <v>3</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36"/>
+      <c r="C10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="15">
-        <v>3</v>
-      </c>
-      <c r="G9" s="15">
-        <v>1</v>
-      </c>
-      <c r="H9" s="15">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F10" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="12" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="36"/>
+      <c r="C11" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>28</v>
@@ -1284,79 +1311,79 @@
         <v>29</v>
       </c>
       <c r="F11" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="11">
-        <v>3</v>
-      </c>
-      <c r="G12" s="11">
-        <v>1</v>
+    <row r="12" spans="2:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36"/>
+      <c r="C12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="29">
+        <v>3</v>
+      </c>
+      <c r="G12" s="29">
+        <v>2</v>
       </c>
       <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35"/>
-      <c r="C13" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="21">
-        <v>3</v>
-      </c>
-      <c r="G13" s="21">
+      <c r="B13" s="37"/>
+      <c r="C13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="20">
+        <v>3</v>
+      </c>
+      <c r="G13" s="20">
         <v>1</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>35</v>
+      <c r="I13" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="G17" s="29" t="s">
+      <c r="E17" s="34"/>
+      <c r="G17" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
@@ -1404,7 +1431,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1434,7 +1461,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16 F3:F13" xr:uid="{947CF420-AD2A-48FA-9957-799D5F7A0144}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F13 G3:G16" xr:uid="{947CF420-AD2A-48FA-9957-799D5F7A0144}">
       <formula1>$E$18:$E$20</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Correciones hechas a partir de la segunda socialización
</commit_message>
<xml_diff>
--- a/2-Analisis_de_Riesgos.xlsx
+++ b/2-Analisis_de_Riesgos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\Ejercicio Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3B1E78-1257-4701-BE6A-C611916D5E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED706FC-CBC2-4003-A86A-F570A5B64E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,7 @@
     <sheet name="Alcance" sheetId="3" r:id="rId4"/>
     <sheet name="Approach" sheetId="4" r:id="rId5"/>
     <sheet name="Casos de Prueba" sheetId="8" r:id="rId6"/>
-    <sheet name="Evidencias" sheetId="6" r:id="rId7"/>
-    <sheet name="Bugtracker" sheetId="7" r:id="rId8"/>
-    <sheet name="Informe de Cierre" sheetId="9" r:id="rId9"/>
+    <sheet name="Bugtracker" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Riesgos!$F$2:$H$2</definedName>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="252">
   <si>
     <t>Riesgo</t>
   </si>
@@ -124,9 +122,6 @@
     <t>Tipo</t>
   </si>
   <si>
-    <t>Existe el riesgo que los 15 días limite no se cumplan dedibo a adiciones en los requisitos del proceso.</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
@@ -205,27 +200,12 @@
     <t>Pruebas funcionales</t>
   </si>
   <si>
-    <t xml:space="preserve">Pruebas de regresion </t>
-  </si>
-  <si>
     <t>HU001 - Consultar Cursos Existentes</t>
   </si>
   <si>
-    <t>Verificación de la disposición de los elementos en pantalla</t>
-  </si>
-  <si>
     <t>Tiempo de visualización</t>
   </si>
   <si>
-    <t>Validación de filtro de busqueda</t>
-  </si>
-  <si>
-    <t>Validación de campo de búsqueda general</t>
-  </si>
-  <si>
-    <t>Verificación de mensajes de validación</t>
-  </si>
-  <si>
     <t>Verificación navegación entre categorías, subcategorias y cursos</t>
   </si>
   <si>
@@ -239,9 +219,6 @@
   </si>
   <si>
     <t>Cierre/Entrega</t>
-  </si>
-  <si>
-    <t>Informe de cierre(reunión de entrega)</t>
   </si>
   <si>
     <t>Entrega de documentación del proyecto</t>
@@ -600,23 +577,6 @@
   </si>
   <si>
     <t>ALCANCE</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-Objetivo
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mitigar la probabilidad de ocurrencia de errores que se puedan presentar en la etapa productiva de la plataforma.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -925,13 +885,7 @@
     <t>Precondiciones</t>
   </si>
   <si>
-    <t>Nombre escenario de prueba</t>
-  </si>
-  <si>
     <t>Data</t>
-  </si>
-  <si>
-    <t>Descripción escenario de prueba</t>
   </si>
   <si>
     <t>Resultado Esperado</t>
@@ -962,14 +916,7 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>SP-000</t>
-  </si>
-  <si>
     <t>Smoke Test</t>
-  </si>
-  <si>
-    <t>Nombre Usuario
-Contraseña</t>
   </si>
   <si>
     <t> - Dar clic en la opción "Universidad Choucair" o "Cursos y Certificaciones" 
@@ -997,9 +944,6 @@
 - Página de categorías</t>
   </si>
   <si>
-    <t>Validación filtro de búsqueda</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -1020,9 +964,6 @@
 - Página de búsqueda</t>
   </si>
   <si>
-    <t>Disposición de los elementos</t>
-  </si>
-  <si>
     <t> - Seleccionar la opción de filtro "Universidad Choucair/ Escuela Técnica/ Automatización"</t>
   </si>
   <si>
@@ -1039,9 +980,6 @@
   </si>
   <si>
     <t>CP-004</t>
-  </si>
-  <si>
-    <t>Validación campo de búsqueda general</t>
   </si>
   <si>
     <t>No ingresar información en el campo</t>
@@ -1057,9 +995,6 @@
     <t>CP-005</t>
   </si>
   <si>
-    <t>""!$%&amp;/</t>
-  </si>
-  <si>
     <t>- Ingresar una palabra con una combinación de caracteres especiales.
 - Presionar tecla enter o dar clic en el botón "Ir"</t>
   </si>
@@ -1070,9 +1005,6 @@
     <t>CP-006</t>
   </si>
   <si>
-    <t>Validación de mensajes</t>
-  </si>
-  <si>
     <t> - Seleccionar la opción de filtro "Universidad Choucair/ Escuela Técnica/ Testing/ Aplicativos"</t>
   </si>
   <si>
@@ -1080,9 +1012,6 @@
   </si>
   <si>
     <t>CP-007</t>
-  </si>
-  <si>
-    <t>Verificación navegación entre categorías, subcategorías y cursos</t>
   </si>
   <si>
     <t> - Dar clic en la opción "Universidad Choucair" o "Cursos y Certificaciones" 
@@ -1090,9 +1019,6 @@
 - Seleccionar subcategoría sí corresponde</t>
   </si>
   <si>
-    <t>- Se deben visualizar las diferentes cursos asociados dependiendo del flujo de búsqueda</t>
-  </si>
-  <si>
     <t>Andrés López
 Camila Jiménez</t>
   </si>
@@ -1106,9 +1032,6 @@
     <t>Retraso en la realización del proceso de pruebas</t>
   </si>
   <si>
-    <t>La aplicacion debe ser de facil entendimiento</t>
-  </si>
-  <si>
     <t>Causa</t>
   </si>
   <si>
@@ -1154,27 +1077,103 @@
     <t>R-003</t>
   </si>
   <si>
+    <t>Cambios en el alcance por adiciones en los requisitos del proceso.</t>
+  </si>
+  <si>
+    <t>La aplicacion debe ser de facil entendimiento - (no es de facil)</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Informe de cierre</t>
+  </si>
+  <si>
+    <t>Reunión de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Categoría
+Curso</t>
+  </si>
+  <si>
+    <t>Paso a Paso</t>
+  </si>
+  <si>
+    <t>Caso de Prueba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP-000
+</t>
+  </si>
+  <si>
+    <t>Consulta de un curso</t>
+  </si>
+  <si>
+    <t>Nombre del escenario</t>
+  </si>
+  <si>
+    <t>Verificación de asociación categoría - curso</t>
+  </si>
+  <si>
+    <t>Verificación del límite de cursos en pantalla</t>
+  </si>
+  <si>
+    <t>Verificación de paginación</t>
+  </si>
+  <si>
+    <t>- Visualizar las diferentes cursos asociados dependiendo del flujo de búsqueda</t>
+  </si>
+  <si>
+    <t>No se muestra un mensaje que evidencie la no existencia de cursos.</t>
+  </si>
+  <si>
+    <t>El tiempo de respuesta para la visualización de los cursos supera el límite establecido</t>
+  </si>
+  <si>
+    <t>Verificación de la disposición de los cursos en pantalla</t>
+  </si>
+  <si>
+    <t>Verificación de la disposición de los cursos</t>
+  </si>
+  <si>
+    <t>Verificación de mensajes de alerta</t>
+  </si>
+  <si>
+    <t>Verificación del filtro de busqueda</t>
+  </si>
+  <si>
+    <t>Verificación del campo de búsqueda general</t>
+  </si>
+  <si>
+    <t>Verificación del filtro de búsqueda</t>
+  </si>
+  <si>
+    <t>Tiempo que tarda en visualizarse los cursos en pantalla</t>
+  </si>
+  <si>
+    <t>Verificación de los cursos que coinciden con la palabra buscada</t>
+  </si>
+  <si>
+    <t>Verificación del campo de búsqueda vacio</t>
+  </si>
+  <si>
+    <t>Verificación de respuestas a fallos</t>
+  </si>
+  <si>
+    <t>Verificación del flujo de navegación entre categorías, subcategorías y cursos</t>
+  </si>
+  <si>
+    <t>Combinación de caracteres especiales</t>
+  </si>
+  <si>
+    <t>Verificación de flujo categoría - subcategpría - curso</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">De acuerdo con los riesgos, para la versión de la plataforma web Choucair Academy.
-Se proyecta una reunión con el cliente para tener un contexto sobre los elementos claves del negocio y los ajustes desarrollados en la plataforma, además, se realizará una revisión y análisis de los requisitos, teniendo en cuenta las restricciones y riesgos del proyecto y producto, se elaborará el diseño de casos de pruebas con el grupo de analistas para determinar las funcionalidades que son determinantes para la comprobación del módulo correspondiente y las diferentes características para validar la calidad del mismo, se establecerá un alcance, approach y se estimará el tiempo necesario para el proceso de pruebas. Teniendo claros estos parámetros se puede iniciar con las pruebas de humo en el aplicativo, lo cual permitirá entender en primera instancia el flujo del módulo y posibles fallos asociados a la aplicación. Posteriormente se realizará la verificación de las funcionalidades que representan un nivel de interacción elevado con el usuario y que determinan el flujo para la consulta de los cursos:
-   1. Verificación del Filtro de búsqueda
-   2. Validación del Campo de búsqueda
-   3. Pantalla de visualización de cursos
-   4. Navegación entre enlaces de categorías, subcategorías y cursos
-   5. Pruebas de regresión.
-Las pruebas están clasificadas de la siguiente manera:
-   - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Smoke Test</t>
+      <t xml:space="preserve">
+Objetivo
+- </t>
     </r>
     <r>
       <rPr>
@@ -1184,73 +1183,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: Verificación básica de los flujos principales del módulo de consultar cursos de la plataforma Choucair Academy, prueba de la lógica de navegación teniendo en cuenta la pantalla principal como el inicio de la búsqueda de los cursos según la categoría principal “Universidad Choucair”, “Cursos y Certificaciones”.
-   - </t>
+      <t>Mitigar la probabilidad de ocurrencia de errores que se puedan presentar en el módulo de búsqueda para cursos existentes</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pruebas de funcionales</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Verificación de las funcionalidades de acuerdo con las características del módulo de consultar cursos, el filtro de los cursos según las categorías y subcategorías y la búsqueda general. Se prueba que no existan fallos en las respuestas que proporcione cada una de las opciones y que la visualización de los cursos o mensajes en la pantalla sean los pertinentes.
-   - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pruebas de desempeño</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Se verifica la calidad de desempeño del aplicativo de acuerdo con la cantidad de cursos visualizados en pantalla y la capacidad del sistema para presentarlos en un tiempo especificado.
-   - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pruebas de seguridad</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Se verifica que en el campo de búsqueda el usuario no puedo ingresar caracteres especiales, teniendo en cuenta que su combinación podría presentar un riesgo de integridad para la información.
+      <t xml:space="preserve">De acuerdo con los riesgos, para la versión de la plataforma web Choucair Academy.
+Se proyecta una reunión con el cliente para tener un contexto sobre los elementos claves del negocio y los ajustes desarrollados en la plataforma, además, se realizará una revisión y análisis de los requisitos, teniendo en cuenta las restricciones y riesgos del proyecto y producto, se elaborará el diseño de casos de pruebas (qué, cuál) con el grupo de analistas para determinar las funcionalidades que son determinantes para la comprobación del módulo correspondiente y las diferentes características para validar la calidad del mismo, se establecerá un alcance, approach y se estimará el tiempo necesario para el proceso de pruebas. Teniendo claros estos parámetros se puede iniciar con las pruebas de humo en el aplicativo, lo cual permitirá entender en primera instancia el flujo del módulo y posibles fallos asociados a la aplicación. Posteriormente se realizará la verificación de las funcionalidades que representan un nivel de interacción elevado con el usuario y que determinan el flujo para la consulta de los cursos:
+   1. Verificación del Filtro de búsqueda
+   2. Validación del Campo de búsqueda
+   3. Pantalla de visualización de cursos
+   4. Navegación entre enlaces de categorías, subcategorías y cursos
+   5. Pruebas de regresión.
+Las pruebas están clasificadas de la siguiente manera:
+   - Smoke Test: Verificación básica de los flujos principales del módulo de consultar cursos de la plataforma Choucair Academy, prueba de la lógica de navegación teniendo en cuenta la pantalla principal como el inicio de la búsqueda de los cursos según la categoría principal “Universidad Choucair”, “Cursos y Certificaciones”.
+   - Pruebas de funcionales: Verificación de las funcionalidades de acuerdo con las características del módulo de consultar cursos, el filtro de los cursos según las categorías y subcategorías y la búsqueda general. Se prueba que no existan fallos en las respuestas que proporcione cada una de las opciones y que la visualización de los cursos o mensajes en la pantalla sean los pertinentes.
+   - Pruebas de Performance: Se recomienda revisar el comportamiento de la plataforma cuando hay un gran número de usuarios ingresando.
+   - Pruebas de seguridad: Se recomienda la realización de estas pruebas sobre el campo de búsqueda, ya que el usuario puede ingresar caracteres especiales, teniendo en cuenta que su combinación podría presentar un riesgo de integridad para la información.
 </t>
     </r>
     <r>
@@ -1262,7 +1211,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Gestión de Pruebas
+      <t xml:space="preserve">
+Gestión de Pruebas
 </t>
     </r>
     <r>
@@ -2091,7 +2041,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2384,6 +2334,30 @@
     <xf numFmtId="0" fontId="27" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2395,6 +2369,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2446,29 +2423,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2528,13 +2484,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>593480</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>146537</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2684,22 +2640,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>299085</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9238</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1" descr="Diagrama&#10;&#10;Descripción generada automáticamente">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C9FB66-9DF8-1954-0A77-B4CD3D1D4528}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDE27A5-F6C8-12BF-BF38-F5662F43FC76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2721,8 +2677,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="57150" y="8858250"/>
-          <a:ext cx="9385935" cy="4972050"/>
+          <a:off x="0" y="8850313"/>
+          <a:ext cx="8391238" cy="4445000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3033,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="C8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3069,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>1</v>
@@ -3085,42 +3041,42 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="126" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="127" t="s">
+      <c r="B3" s="112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="128" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" s="128" t="s">
-        <v>228</v>
-      </c>
-      <c r="F3" s="129">
+      <c r="D3" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="102">
         <v>2</v>
       </c>
-      <c r="G3" s="129">
+      <c r="G3" s="102">
         <v>1</v>
       </c>
-      <c r="H3" s="129">
+      <c r="H3" s="102">
         <f>F3*G3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="130" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="104"/>
-      <c r="C4" s="127" t="s">
+      <c r="I3" s="103" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="113"/>
+      <c r="C4" s="100" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>220</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="F4" s="11">
         <v>3</v>
@@ -3133,19 +3089,19 @@
         <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="104"/>
-      <c r="C5" s="127" t="s">
-        <v>239</v>
+      <c r="B5" s="113"/>
+      <c r="C5" s="100" t="s">
+        <v>219</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="131" t="s">
-        <v>33</v>
+        <v>203</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="F5" s="11">
         <v>2</v>
@@ -3158,19 +3114,19 @@
         <v>2</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
-      <c r="C6" s="127" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="114"/>
+      <c r="C6" s="100" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="F6" s="14">
         <v>3</v>
@@ -3183,46 +3139,46 @@
         <v>6</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="126" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="127" t="s">
+      <c r="B7" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="128" t="s">
-        <v>224</v>
-      </c>
-      <c r="E7" s="132" t="s">
-        <v>235</v>
-      </c>
-      <c r="F7" s="129">
+      <c r="D7" s="101" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="104" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="102">
         <v>3</v>
       </c>
-      <c r="G7" s="129">
+      <c r="G7" s="102">
         <v>1</v>
       </c>
-      <c r="H7" s="129">
+      <c r="H7" s="102">
         <f t="shared" ref="H7:H11" si="0">F7*G7</f>
         <v>3</v>
       </c>
-      <c r="I7" s="133" t="s">
-        <v>28</v>
+      <c r="I7" s="105" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="104"/>
-      <c r="C8" s="127" t="s">
+      <c r="B8" s="113"/>
+      <c r="C8" s="100" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="F8" s="11">
         <v>2</v>
@@ -3239,15 +3195,15 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="104"/>
-      <c r="C9" s="127" t="s">
+      <c r="B9" s="113"/>
+      <c r="C9" s="100" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="F9" s="11">
         <v>3</v>
@@ -3264,15 +3220,15 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="104"/>
-      <c r="C10" s="127" t="s">
+      <c r="B10" s="113"/>
+      <c r="C10" s="100" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="22">
         <v>3</v>
@@ -3285,19 +3241,19 @@
         <v>6</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="105"/>
+      <c r="B11" s="114"/>
       <c r="C11" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="F11" s="14">
         <v>3</v>
@@ -3315,14 +3271,14 @@
     </row>
     <row r="15" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="103"/>
-      <c r="G15" s="100" t="s">
+      <c r="E15" s="111"/>
+      <c r="G15" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="101"/>
+      <c r="H15" s="109"/>
     </row>
     <row r="16" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -3410,10 +3366,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57352B70-E1DD-4553-B340-6DCB8A3F1E05}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,24 +3384,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -3457,7 +3413,7 @@
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="33">
         <v>3</v>
@@ -3473,7 +3429,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="33">
         <v>3</v>
@@ -3496,7 +3452,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="37"/>
@@ -3508,7 +3464,7 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="33">
         <v>3</v>
@@ -3531,7 +3487,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="37"/>
@@ -3543,7 +3499,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="33">
         <v>3</v>
@@ -3559,7 +3515,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="33">
         <v>3</v>
@@ -3575,7 +3531,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="33">
         <v>3</v>
@@ -3591,7 +3547,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="33">
         <v>3</v>
@@ -3607,174 +3563,144 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="39">
-        <f>SUM(E15:E17)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="33">
-        <v>2</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="35">
-        <f>+B15*D15</f>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36">
+        <f>SUM(C16:C21)</f>
+        <v>10</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="39">
+        <f>SUM(E16:E21)</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="33">
-        <v>2</v>
-      </c>
-      <c r="C16" s="33"/>
       <c r="D16" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" ref="E16:E21" si="1">C16*D16</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33">
         <v>1</v>
       </c>
-      <c r="E16" s="35">
-        <f t="shared" ref="E16:E17" si="1">+B16*D16</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="33">
-        <v>2</v>
-      </c>
-      <c r="C17" s="33"/>
       <c r="D17" s="33">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E17" s="35">
         <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36">
-        <f>SUM(C19:C24)</f>
-        <v>10</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="39">
-        <f>SUM(E19:E24)</f>
-        <v>3.8</v>
+      <c r="D18" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="35">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
-        <v>55</v>
+      <c r="A19" s="43" t="s">
+        <v>241</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="33">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="35">
-        <f t="shared" ref="E19:E24" si="2">C19*D19</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>56</v>
+        <v>239</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33">
         <v>1</v>
       </c>
       <c r="D20" s="33">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="35">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="33">
         <v>2</v>
       </c>
       <c r="D21" s="33">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="35">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>58</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="43"/>
       <c r="B22" s="33"/>
-      <c r="C22" s="33">
-        <v>3</v>
-      </c>
-      <c r="D22" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="35">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>59</v>
-      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
       <c r="B23" s="33"/>
-      <c r="C23" s="33">
-        <v>1</v>
-      </c>
-      <c r="D23" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="E23" s="35">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>60</v>
-      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="35"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
       <c r="B24" s="33"/>
-      <c r="C24" s="33">
-        <v>2</v>
-      </c>
-      <c r="D24" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="35">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="35"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
@@ -3785,24 +3711,26 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
       <c r="E26" s="45">
         <f>SUM(E27:E29)</f>
-        <v>7</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="33">
         <v>2</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="33">
+        <v>1</v>
+      </c>
       <c r="D27" s="33">
         <v>0.5</v>
       </c>
@@ -3813,51 +3741,55 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="33"/>
+        <v>56</v>
+      </c>
+      <c r="B28" s="33">
+        <v>3</v>
+      </c>
       <c r="C28" s="33">
-        <v>6</v>
+        <v>3.3</v>
       </c>
       <c r="D28" s="46">
         <v>0.5</v>
       </c>
       <c r="E28" s="47">
         <f>C28*D28</f>
-        <v>3</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B29" s="33">
         <v>2</v>
       </c>
-      <c r="C29" s="33"/>
+      <c r="C29" s="33">
+        <v>2</v>
+      </c>
       <c r="D29" s="33">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="35">
-        <f t="shared" ref="E29" si="3">+B29*D29</f>
-        <v>3</v>
+        <f t="shared" ref="E29" si="2">+B29*D29</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
       <c r="E30" s="39">
-        <f>SUM(E31:E32)</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <f>SUM(E31:E34)</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
       <c r="B31" s="33">
         <v>3</v>
@@ -3871,133 +3803,160 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="B32" s="33">
         <v>3</v>
       </c>
-      <c r="C32" s="33"/>
+      <c r="C32" s="33">
+        <v>3</v>
+      </c>
       <c r="D32" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="E32" s="35">
+        <f>C32*D32*B32</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="35"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="33">
+        <v>3</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33">
         <v>0.5</v>
       </c>
-      <c r="E32" s="35">
-        <f>B32*D32</f>
+      <c r="E34" s="35">
+        <f>B34*D34</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="45">
-        <f>SUM(E2,E6,E9,E14,E18,E26,E30)</f>
-        <v>35.299999999999997</v>
-      </c>
-      <c r="F33" s="51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-    </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-    </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="45">
+        <f>SUM(E2,E6,E9,E14,E15,E26,E30)</f>
+        <v>29.2</v>
+      </c>
+      <c r="F35" s="51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
-      <c r="C36" s="53">
-        <f>E33*E36</f>
-        <v>3.8829999999999996</v>
-      </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="52"/>
+    </row>
+    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="52"/>
+      <c r="C38" s="53">
+        <f>E35*E38</f>
+        <v>3.2119999999999997</v>
+      </c>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55">
         <f>'Factor de Ajuste'!B16</f>
         <v>0.11</v>
       </c>
-      <c r="F36" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="C37" s="57">
-        <f>E33+C36</f>
-        <v>39.183</v>
-      </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="52"/>
+      <c r="C39" s="57">
+        <f>E35+C38</f>
+        <v>32.411999999999999</v>
+      </c>
+      <c r="D39" s="58"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="56" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="106" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="106"/>
-      <c r="D40" s="61">
-        <v>3</v>
-      </c>
+      <c r="A40" s="52"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
-      <c r="B41" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="106"/>
-      <c r="D41" s="62">
-        <v>9</v>
-      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
-      <c r="B42" s="106" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="106"/>
-      <c r="D42" s="62">
-        <f>D41*D40</f>
-        <v>27</v>
-      </c>
-      <c r="F42" t="s">
-        <v>75</v>
+      <c r="A42" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="115"/>
+      <c r="D42" s="61">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="52"/>
-      <c r="B43" s="106" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="106"/>
-      <c r="D43" s="63">
-        <f>C37/D42</f>
-        <v>1.4512222222222222</v>
+      <c r="B43" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="115"/>
+      <c r="D43" s="62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="52"/>
+      <c r="B44" s="115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="115"/>
+      <c r="D44" s="57">
+        <f>C39/D42</f>
+        <v>10.804</v>
+      </c>
+      <c r="F44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="52"/>
+      <c r="B45" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="115"/>
+      <c r="D45" s="63">
+        <f>D44/D43</f>
+        <v>1.2004444444444444</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4008,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897B68CF-C3FB-42BA-9434-9C60A06D8598}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,25 +3990,25 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C2" s="64"/>
-      <c r="D2" s="107" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="109"/>
+      <c r="D2" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="118"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B3" s="67">
         <v>0</v>
@@ -4058,54 +4017,54 @@
       <c r="D3" s="68">
         <v>1</v>
       </c>
-      <c r="E3" s="110" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="109"/>
+      <c r="E3" s="119" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="118"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B4" s="67">
         <v>0.01</v>
       </c>
       <c r="C4" s="64"/>
-      <c r="D4" s="111">
+      <c r="D4" s="120">
         <v>2</v>
       </c>
-      <c r="E4" s="113" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="114"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="115"/>
+      <c r="E4" s="122" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="124"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B5" s="67">
         <v>0.01</v>
       </c>
       <c r="C5" s="64"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="118"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B6" s="67">
         <v>0.01</v>
@@ -4114,18 +4073,18 @@
       <c r="D6" s="68">
         <v>3</v>
       </c>
-      <c r="E6" s="110" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="109"/>
+      <c r="E6" s="119" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="118"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B7" s="67">
         <v>0</v>
@@ -4141,7 +4100,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B8" s="67">
         <v>0.02</v>
@@ -4157,7 +4116,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B9" s="67">
         <v>0</v>
@@ -4173,7 +4132,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B10" s="67">
         <v>0.01</v>
@@ -4189,7 +4148,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="66" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B11" s="67">
         <v>0.01</v>
@@ -4205,7 +4164,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B12" s="67">
         <v>0.01</v>
@@ -4221,7 +4180,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B13" s="67">
         <v>0</v>
@@ -4237,7 +4196,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B14" s="67">
         <v>0.01</v>
@@ -4253,7 +4212,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B15" s="67">
         <v>0.02</v>
@@ -4269,17 +4228,17 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B16" s="70">
         <f>SUM(B3:B15)</f>
         <v>0.11</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D16" s="71" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E16" s="64"/>
       <c r="F16" s="64"/>
@@ -4292,10 +4251,10 @@
       <c r="A17" s="64"/>
       <c r="B17" s="64"/>
       <c r="C17" s="72" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D17" s="72" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E17" s="64"/>
       <c r="F17" s="64"/>
@@ -4320,506 +4279,506 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F0E5-6471-4CC4-B93C-4C0C792F046B}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="A39" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="129" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="130" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="130"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="130"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="130"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="130"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="131" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="132"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="132"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="132"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="132"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="132"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="132"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="132"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="132"/>
+      <c r="B14" s="132"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="132"/>
+      <c r="B15" s="132"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="132"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="132"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="132"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="132"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="132"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="132"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="132"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="132"/>
+      <c r="F20" s="132"/>
+      <c r="G20" s="132"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="132"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="132"/>
+      <c r="G21" s="132"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="132"/>
+      <c r="B22" s="132"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="132"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="132"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="132"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="132"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
+      <c r="G24" s="132"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="132"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="132"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="132"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="132"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="132"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="132"/>
+      <c r="G27" s="132"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="132"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="132"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="132"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="132"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="132"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="129" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="129" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="129"/>
+      <c r="G32" s="129"/>
+    </row>
+    <row r="33" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="128" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="128"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="128"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
+      <c r="E34" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="133"/>
+      <c r="G34" s="133"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="134" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="134"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="133"/>
+      <c r="G35" s="133"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="B36" s="134"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="133"/>
+      <c r="G36" s="133"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="B37" s="128"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
+      <c r="E37" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="133"/>
+      <c r="G37" s="133"/>
+    </row>
+    <row r="38" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="128" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="123"/>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="123"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="123"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="123"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="123"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="123"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="123"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="123"/>
-      <c r="B15" s="123"/>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="123"/>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="123"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="123"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="123"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="123"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="123"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="123"/>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="123"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="123"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="123"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="123"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="123"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="123"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="123"/>
-      <c r="B28" s="123"/>
-      <c r="C28" s="123"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="123"/>
-      <c r="B29" s="123"/>
-      <c r="C29" s="123"/>
-      <c r="D29" s="123"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="123"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="123"/>
-      <c r="B30" s="123"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
-      <c r="B31" s="123"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="123"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="120"/>
-      <c r="C32" s="120"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="120" t="s">
+      <c r="B38" s="128"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="133" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="120"/>
-      <c r="G32" s="120"/>
-    </row>
-    <row r="33" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="119" t="s">
+      <c r="F38" s="133"/>
+      <c r="G38" s="133"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="119"/>
-      <c r="C33" s="119"/>
-      <c r="D33" s="119"/>
-      <c r="E33" s="124" t="s">
-        <v>112</v>
-      </c>
-      <c r="F33" s="124"/>
-      <c r="G33" s="124"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="119" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="119"/>
-      <c r="C34" s="119"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="125" t="s">
-        <v>108</v>
-      </c>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="124"/>
-      <c r="G35" s="124"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="125" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="124"/>
-      <c r="G36" s="124"/>
-    </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="119" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="119"/>
-      <c r="E37" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="124"/>
-      <c r="G37" s="124"/>
-    </row>
-    <row r="38" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="119"/>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="124" t="s">
-        <v>113</v>
-      </c>
-      <c r="F38" s="124"/>
-      <c r="G38" s="124"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="119" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="125"/>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="125"/>
-      <c r="F39" s="125"/>
-      <c r="G39" s="125"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="125"/>
-      <c r="B40" s="125"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="125"/>
-      <c r="G40" s="125"/>
+      <c r="A40" s="134"/>
+      <c r="B40" s="134"/>
+      <c r="C40" s="134"/>
+      <c r="D40" s="134"/>
+      <c r="E40" s="134"/>
+      <c r="F40" s="134"/>
+      <c r="G40" s="134"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="125"/>
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="125"/>
+      <c r="A41" s="134"/>
+      <c r="B41" s="134"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="134"/>
+      <c r="F41" s="134"/>
+      <c r="G41" s="134"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="125"/>
-      <c r="B42" s="125"/>
-      <c r="C42" s="125"/>
-      <c r="D42" s="125"/>
-      <c r="E42" s="125"/>
-      <c r="F42" s="125"/>
-      <c r="G42" s="125"/>
+      <c r="A42" s="134"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="134"/>
+      <c r="F42" s="134"/>
+      <c r="G42" s="134"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="125"/>
-      <c r="B43" s="125"/>
-      <c r="C43" s="125"/>
-      <c r="D43" s="125"/>
-      <c r="E43" s="125"/>
-      <c r="F43" s="125"/>
-      <c r="G43" s="125"/>
+      <c r="A43" s="134"/>
+      <c r="B43" s="134"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="134"/>
+      <c r="G43" s="134"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="125"/>
-      <c r="B44" s="125"/>
-      <c r="C44" s="125"/>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="125"/>
+      <c r="A44" s="134"/>
+      <c r="B44" s="134"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
+      <c r="E44" s="134"/>
+      <c r="F44" s="134"/>
+      <c r="G44" s="134"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="125"/>
-      <c r="B45" s="125"/>
-      <c r="C45" s="125"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="125"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="125"/>
+      <c r="A45" s="134"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="134"/>
+      <c r="F45" s="134"/>
+      <c r="G45" s="134"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="125"/>
-      <c r="B46" s="125"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="125"/>
-      <c r="E46" s="125"/>
-      <c r="F46" s="125"/>
-      <c r="G46" s="125"/>
+      <c r="A46" s="134"/>
+      <c r="B46" s="134"/>
+      <c r="C46" s="134"/>
+      <c r="D46" s="134"/>
+      <c r="E46" s="134"/>
+      <c r="F46" s="134"/>
+      <c r="G46" s="134"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="125"/>
-      <c r="B47" s="125"/>
-      <c r="C47" s="125"/>
-      <c r="D47" s="125"/>
-      <c r="E47" s="125"/>
-      <c r="F47" s="125"/>
-      <c r="G47" s="125"/>
+      <c r="A47" s="134"/>
+      <c r="B47" s="134"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="134"/>
+      <c r="F47" s="134"/>
+      <c r="G47" s="134"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="125"/>
-      <c r="B48" s="125"/>
-      <c r="C48" s="125"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="125"/>
-      <c r="F48" s="125"/>
-      <c r="G48" s="125"/>
+      <c r="A48" s="134"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="134"/>
+      <c r="F48" s="134"/>
+      <c r="G48" s="134"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="125"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="125"/>
-      <c r="D49" s="125"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
-      <c r="G49" s="125"/>
+      <c r="A49" s="134"/>
+      <c r="B49" s="134"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134"/>
+      <c r="G49" s="134"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="125"/>
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
-      <c r="D50" s="125"/>
-      <c r="E50" s="125"/>
-      <c r="F50" s="125"/>
-      <c r="G50" s="125"/>
+      <c r="A50" s="134"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="134"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="134"/>
+      <c r="F50" s="134"/>
+      <c r="G50" s="134"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="125"/>
-      <c r="B51" s="125"/>
-      <c r="C51" s="125"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
-      <c r="G51" s="125"/>
+      <c r="A51" s="134"/>
+      <c r="B51" s="134"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -4851,455 +4810,455 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60306786-1A89-4F4E-8933-14BCEF41428F}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A34" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
+      <c r="A1" s="129" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
+      <c r="A2" s="135" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
+      <c r="A3" s="135"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+      <c r="A4" s="135"/>
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
+      <c r="A5" s="135"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="135"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
+      <c r="A9" s="135"/>
+      <c r="B9" s="135"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="I9" s="135"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="119"/>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="135"/>
+      <c r="C10" s="135"/>
+      <c r="D10" s="135"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="119"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
+      <c r="A11" s="135"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="135"/>
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="119"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="119"/>
-      <c r="I12" s="119"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="135"/>
+      <c r="C12" s="135"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
-      <c r="B13" s="119"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="119"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="119"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="119"/>
+      <c r="A13" s="135"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="135"/>
+      <c r="D13" s="135"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="135"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="119"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
+      <c r="A14" s="135"/>
+      <c r="B14" s="135"/>
+      <c r="C14" s="135"/>
+      <c r="D14" s="135"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="135"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="119"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="119"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="135"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="119"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="119"/>
-      <c r="H16" s="119"/>
-      <c r="I16" s="119"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="135"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="119"/>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
-      <c r="G17" s="119"/>
-      <c r="H17" s="119"/>
-      <c r="I17" s="119"/>
+      <c r="A17" s="135"/>
+      <c r="B17" s="135"/>
+      <c r="C17" s="135"/>
+      <c r="D17" s="135"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="135"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="135"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="119"/>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
+      <c r="A18" s="135"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="119"/>
-      <c r="B19" s="119"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="119"/>
-      <c r="G19" s="119"/>
-      <c r="H19" s="119"/>
-      <c r="I19" s="119"/>
+      <c r="A19" s="135"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="135"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="135"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="119"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="119"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="119"/>
-      <c r="I20" s="119"/>
+      <c r="A20" s="135"/>
+      <c r="B20" s="135"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="119"/>
-      <c r="B21" s="119"/>
-      <c r="C21" s="119"/>
-      <c r="D21" s="119"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="119"/>
-      <c r="H21" s="119"/>
-      <c r="I21" s="119"/>
+      <c r="A21" s="135"/>
+      <c r="B21" s="135"/>
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="135"/>
+      <c r="I21" s="135"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="119"/>
-      <c r="B22" s="119"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="119"/>
+      <c r="A22" s="135"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="135"/>
+      <c r="D22" s="135"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="135"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="119"/>
-      <c r="B23" s="119"/>
-      <c r="C23" s="119"/>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="119"/>
-      <c r="H23" s="119"/>
-      <c r="I23" s="119"/>
+      <c r="A23" s="135"/>
+      <c r="B23" s="135"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="135"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="135"/>
+      <c r="H23" s="135"/>
+      <c r="I23" s="135"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="119"/>
-      <c r="B24" s="119"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="119"/>
-      <c r="H24" s="119"/>
-      <c r="I24" s="119"/>
+      <c r="A24" s="135"/>
+      <c r="B24" s="135"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="119"/>
-      <c r="B25" s="119"/>
-      <c r="C25" s="119"/>
-      <c r="D25" s="119"/>
-      <c r="E25" s="119"/>
-      <c r="F25" s="119"/>
-      <c r="G25" s="119"/>
-      <c r="H25" s="119"/>
-      <c r="I25" s="119"/>
+      <c r="A25" s="135"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="135"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="119"/>
-      <c r="B26" s="119"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="119"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="119"/>
-      <c r="I26" s="119"/>
+      <c r="A26" s="135"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
+      <c r="F26" s="135"/>
+      <c r="G26" s="135"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="135"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="119"/>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="119"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="135"/>
+      <c r="I27" s="135"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="119"/>
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="119"/>
+      <c r="A28" s="135"/>
+      <c r="B28" s="135"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="135"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="135"/>
+      <c r="H28" s="135"/>
+      <c r="I28" s="135"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="119"/>
-      <c r="B29" s="119"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="119"/>
-      <c r="I29" s="119"/>
+      <c r="A29" s="135"/>
+      <c r="B29" s="135"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="135"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="135"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="119"/>
-      <c r="B30" s="119"/>
-      <c r="C30" s="119"/>
-      <c r="D30" s="119"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="119"/>
-      <c r="I30" s="119"/>
+      <c r="A30" s="135"/>
+      <c r="B30" s="135"/>
+      <c r="C30" s="135"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="135"/>
+      <c r="H30" s="135"/>
+      <c r="I30" s="135"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="119"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="119"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="119"/>
+      <c r="A31" s="135"/>
+      <c r="B31" s="135"/>
+      <c r="C31" s="135"/>
+      <c r="D31" s="135"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="135"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="135"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="119"/>
-      <c r="B32" s="119"/>
-      <c r="C32" s="119"/>
-      <c r="D32" s="119"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="119"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="119"/>
-      <c r="I32" s="119"/>
+      <c r="A32" s="135"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="119"/>
-      <c r="B33" s="119"/>
-      <c r="C33" s="119"/>
-      <c r="D33" s="119"/>
-      <c r="E33" s="119"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="119"/>
-      <c r="I33" s="119"/>
+      <c r="A33" s="135"/>
+      <c r="B33" s="135"/>
+      <c r="C33" s="135"/>
+      <c r="D33" s="135"/>
+      <c r="E33" s="135"/>
+      <c r="F33" s="135"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="135"/>
+      <c r="I33" s="135"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="119"/>
-      <c r="B34" s="119"/>
-      <c r="C34" s="119"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="119"/>
+      <c r="A34" s="135"/>
+      <c r="B34" s="135"/>
+      <c r="C34" s="135"/>
+      <c r="D34" s="135"/>
+      <c r="E34" s="135"/>
+      <c r="F34" s="135"/>
+      <c r="G34" s="135"/>
+      <c r="H34" s="135"/>
+      <c r="I34" s="135"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="119"/>
-      <c r="B35" s="119"/>
-      <c r="C35" s="119"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="119"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="119"/>
-      <c r="I35" s="119"/>
+      <c r="A35" s="135"/>
+      <c r="B35" s="135"/>
+      <c r="C35" s="135"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="135"/>
+      <c r="F35" s="135"/>
+      <c r="G35" s="135"/>
+      <c r="H35" s="135"/>
+      <c r="I35" s="135"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="119"/>
-      <c r="B36" s="119"/>
-      <c r="C36" s="119"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="119"/>
+      <c r="A36" s="135"/>
+      <c r="B36" s="135"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="135"/>
+      <c r="E36" s="135"/>
+      <c r="F36" s="135"/>
+      <c r="G36" s="135"/>
+      <c r="H36" s="135"/>
+      <c r="I36" s="135"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="119"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="119"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="119"/>
-      <c r="H37" s="119"/>
-      <c r="I37" s="119"/>
+      <c r="A37" s="135"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="135"/>
+      <c r="G37" s="135"/>
+      <c r="H37" s="135"/>
+      <c r="I37" s="135"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="119"/>
-      <c r="B38" s="119"/>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="119"/>
+      <c r="A38" s="135"/>
+      <c r="B38" s="135"/>
+      <c r="C38" s="135"/>
+      <c r="D38" s="135"/>
+      <c r="E38" s="135"/>
+      <c r="F38" s="135"/>
+      <c r="G38" s="135"/>
+      <c r="H38" s="135"/>
+      <c r="I38" s="135"/>
     </row>
     <row r="39" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="119"/>
-      <c r="B39" s="119"/>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="119"/>
+      <c r="A39" s="135"/>
+      <c r="B39" s="135"/>
+      <c r="C39" s="135"/>
+      <c r="D39" s="135"/>
+      <c r="E39" s="135"/>
+      <c r="F39" s="135"/>
+      <c r="G39" s="135"/>
+      <c r="H39" s="135"/>
+      <c r="I39" s="135"/>
     </row>
     <row r="40" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="119"/>
-      <c r="B40" s="119"/>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119"/>
+      <c r="A40" s="135"/>
+      <c r="B40" s="135"/>
+      <c r="C40" s="135"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="135"/>
+      <c r="G40" s="135"/>
+      <c r="H40" s="135"/>
+      <c r="I40" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5307,393 +5266,423 @@
     <mergeCell ref="A2:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB046DB-1D33-48E7-86E9-051E6AFDCBB5}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="85" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="86" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="M1" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="N1" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="O1" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="85" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="85" t="s">
+      <c r="D2" s="107" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="85" t="s">
+      <c r="H2" s="91" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="I2" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="J2" s="95">
+        <v>44971</v>
+      </c>
+      <c r="K2" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="93" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="O2" s="96"/>
+    </row>
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="87" t="s">
+      <c r="B3" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="107" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="91" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="F3" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="N1" s="89" t="s">
+      <c r="G3" s="93" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="H3" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="91" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="90" t="s">
+      <c r="I3" s="96" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="95">
+        <v>44971</v>
+      </c>
+      <c r="K3" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="93" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="M3" s="93" t="s">
+        <v>181</v>
+      </c>
+      <c r="N3" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O3" s="99" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="B4" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="91" t="s">
+      <c r="F4" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="94" t="s">
+      <c r="H4" s="98" t="s">
         <v>185</v>
       </c>
-      <c r="I2" s="95">
+      <c r="I4" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="J4" s="95">
         <v>44971</v>
       </c>
-      <c r="J2" s="96" t="s">
+      <c r="K4" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O4" s="99"/>
+    </row>
+    <row r="5" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="93" t="s">
+      <c r="B5" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="107" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="N2" s="96"/>
-    </row>
-    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="I5" s="96" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="95">
+        <v>44971</v>
+      </c>
+      <c r="K5" s="93" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="91" t="s">
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O5" s="99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="97" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="B6" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="107" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="93" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="G6" s="98" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="H6" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="98" t="s">
+      <c r="I6" s="96" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="95">
+        <v>44971</v>
+      </c>
+      <c r="K6" s="93" t="s">
+        <v>188</v>
+      </c>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O6" s="99" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="97" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="96" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" s="95">
+      <c r="B7" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="107" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="98" t="s">
+        <v>194</v>
+      </c>
+      <c r="H7" s="98" t="s">
+        <v>195</v>
+      </c>
+      <c r="I7" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="95">
+        <v>44973</v>
+      </c>
+      <c r="K7" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="93"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O7" s="99"/>
+    </row>
+    <row r="8" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="97" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="107" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="93" t="s">
+        <v>197</v>
+      </c>
+      <c r="H8" s="98" t="s">
+        <v>198</v>
+      </c>
+      <c r="I8" s="96" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="95">
         <v>44971</v>
       </c>
-      <c r="J3" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="K3" s="93" t="s">
-        <v>194</v>
-      </c>
-      <c r="L3" s="93" t="s">
-        <v>194</v>
-      </c>
-      <c r="M3" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N3" s="99" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="91" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="93" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" s="93" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4" s="93" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="98" t="s">
+      <c r="K8" s="93" t="s">
+        <v>188</v>
+      </c>
+      <c r="L8" s="93"/>
+      <c r="M8" s="93"/>
+      <c r="N8" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O8" s="99" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="96" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="95">
+      <c r="B9" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="93" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9" s="107" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="93" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="93" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" s="91" t="s">
+        <v>234</v>
+      </c>
+      <c r="I9" s="94" t="s">
+        <v>201</v>
+      </c>
+      <c r="J9" s="95">
         <v>44971</v>
       </c>
-      <c r="J4" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N4" s="99"/>
-    </row>
-    <row r="5" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="91" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="93" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="H5" s="96" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="95">
-        <v>44971</v>
-      </c>
-      <c r="J5" s="93" t="s">
-        <v>202</v>
-      </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N5" s="99" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="93" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6" s="93" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="98" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6" s="98" t="s">
-        <v>207</v>
-      </c>
-      <c r="H6" s="96" t="s">
-        <v>143</v>
-      </c>
-      <c r="I6" s="95">
-        <v>44971</v>
-      </c>
-      <c r="J6" s="93" t="s">
-        <v>202</v>
-      </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N6" s="99" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
-        <v>208</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="93" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" s="93" t="s">
-        <v>209</v>
-      </c>
-      <c r="F7" s="98" t="s">
-        <v>210</v>
-      </c>
-      <c r="G7" s="98" t="s">
-        <v>211</v>
-      </c>
-      <c r="H7" s="96" t="s">
-        <v>136</v>
-      </c>
-      <c r="I7" s="95">
-        <v>44973</v>
-      </c>
-      <c r="J7" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N7" s="99"/>
-    </row>
-    <row r="8" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="93" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="93" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="H8" s="96" t="s">
-        <v>136</v>
-      </c>
-      <c r="I8" s="95">
-        <v>44971</v>
-      </c>
-      <c r="J8" s="93" t="s">
-        <v>202</v>
-      </c>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N8" s="99" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
-        <v>216</v>
-      </c>
-      <c r="B9" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="91" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="93" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="93" t="s">
-        <v>218</v>
-      </c>
-      <c r="G9" s="91" t="s">
-        <v>219</v>
-      </c>
-      <c r="H9" s="94" t="s">
-        <v>220</v>
-      </c>
-      <c r="I9" s="95">
-        <v>44971</v>
-      </c>
-      <c r="J9" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="K9" s="93"/>
+      <c r="K9" s="93" t="s">
+        <v>174</v>
+      </c>
       <c r="L9" s="93"/>
-      <c r="M9" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="N9" s="99"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93" t="s">
+        <v>175</v>
+      </c>
+      <c r="O9" s="99"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J9 M2:M9" xr:uid="{F4EFF9D8-062C-4EA1-AC9D-88F3CAF300AC}">
-      <formula1>$AH$3:$AH$9</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K9 N2:N9" xr:uid="{F4EFF9D8-062C-4EA1-AC9D-88F3CAF300AC}">
+      <formula1>$AI$3:$AI$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5701,25 +5690,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B785F1C0-1D54-444A-80D5-CB16A1F30C40}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9B0E9A-F39F-4AAC-8A39-110191E12869}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5728,13 +5703,13 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.42578125" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -5745,78 +5720,78 @@
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E1" s="73" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H1" s="73" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I1" s="73" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J1" s="73" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="K1" s="73" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L1" s="73" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="M1" s="73" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="73" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="O1" s="73" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="P1" s="73" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="73" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C2" s="74" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>133</v>
+        <v>236</v>
       </c>
       <c r="E2" s="77" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F2" s="78" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H2" s="78"/>
       <c r="I2" s="79">
@@ -5825,7 +5800,7 @@
       <c r="J2" s="79"/>
       <c r="K2" s="79"/>
       <c r="L2" s="80" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="M2" s="78">
         <v>2</v>
@@ -5837,34 +5812,34 @@
         <v>2</v>
       </c>
       <c r="P2" s="78" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="Q2" s="74"/>
     </row>
     <row r="3" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E3" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="78" t="s">
-        <v>142</v>
-      </c>
       <c r="G3" s="74" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H3" s="78" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I3" s="79">
         <v>44971</v>
@@ -5876,7 +5851,7 @@
         <v>44974</v>
       </c>
       <c r="L3" s="80" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="M3" s="78">
         <v>1</v>
@@ -5888,31 +5863,31 @@
         <v>2</v>
       </c>
       <c r="P3" s="78" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="Q3" s="74"/>
     </row>
     <row r="4" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>148</v>
+        <v>235</v>
       </c>
       <c r="E4" s="77" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F4" s="78" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H4" s="78"/>
       <c r="I4" s="79">
@@ -5921,7 +5896,7 @@
       <c r="J4" s="79"/>
       <c r="K4" s="79"/>
       <c r="L4" s="80" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="M4" s="78">
         <v>1</v>
@@ -5933,36 +5908,36 @@
         <v>2</v>
       </c>
       <c r="P4" s="78" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="Q4" s="82" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D5" s="83" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F5" s="78" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H5" s="78" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I5" s="79">
         <v>44973</v>
@@ -5974,7 +5949,7 @@
         <v>44977</v>
       </c>
       <c r="L5" s="80" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="M5" s="78">
         <v>1</v>
@@ -5986,33 +5961,33 @@
         <v>2</v>
       </c>
       <c r="P5" s="78" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="Q5" s="83" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B6" s="75" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D6" s="83" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F6" s="78" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G6" s="74" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H6" s="78"/>
       <c r="I6" s="79">
@@ -6021,7 +5996,7 @@
       <c r="J6" s="79"/>
       <c r="K6" s="79"/>
       <c r="L6" s="80" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="M6" s="78">
         <v>4</v>
@@ -6033,10 +6008,10 @@
         <v>4</v>
       </c>
       <c r="P6" s="78" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="Q6" s="83" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -6053,16 +6028,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E813C4-8121-4B97-9B4E-5CAA81AC2662}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>